<commit_message>
Help room begin. Todo: Finish help room, then first room
</commit_message>
<xml_diff>
--- a/doc/大作业自评表.xlsx
+++ b/doc/大作业自评表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\程序设计基础\2024013355_黄添豪\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B220B2-D1C9-451D-ACF3-129B707AF00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B63712-CDDC-4D62-9522-5786FADB5E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,6 +840,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -854,27 +875,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1175,17 +1175,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -1205,10 +1205,10 @@
       <c r="A3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="39"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="28"/>
       <c r="F3" s="30"/>
       <c r="G3" s="27"/>
@@ -1230,25 +1230,25 @@
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37" t="s">
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="31" t="s">
         <v>1</v>
       </c>
@@ -1288,7 +1288,9 @@
       <c r="D8" s="15">
         <v>1</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="18">
+        <v>1</v>
+      </c>
       <c r="F8" s="19" t="s">
         <v>87</v>
       </c>
@@ -1310,7 +1312,9 @@
       <c r="D9" s="15">
         <v>2</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18">
+        <v>2</v>
+      </c>
       <c r="F9" s="18" t="s">
         <v>89</v>
       </c>
@@ -1334,7 +1338,9 @@
       <c r="D10" s="18">
         <v>2</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="18">
+        <v>2</v>
+      </c>
       <c r="F10" s="18"/>
       <c r="G10" s="3"/>
       <c r="H10" s="15"/>
@@ -1440,7 +1446,9 @@
       <c r="D15" s="15">
         <v>3</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="18">
+        <v>3</v>
+      </c>
       <c r="F15" s="18" t="s">
         <v>75</v>
       </c>
@@ -1490,7 +1498,9 @@
       <c r="D17" s="15">
         <v>3</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="18">
+        <v>3</v>
+      </c>
       <c r="F17" s="19" t="s">
         <v>78</v>
       </c>
@@ -1514,7 +1524,9 @@
       <c r="D18" s="15">
         <v>3</v>
       </c>
-      <c r="E18" s="18"/>
+      <c r="E18" s="18">
+        <v>3</v>
+      </c>
       <c r="F18" s="19" t="s">
         <v>40</v>
       </c>
@@ -1536,7 +1548,9 @@
       <c r="D19" s="15">
         <v>3</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="18">
+        <v>3</v>
+      </c>
       <c r="F19" s="18" t="s">
         <v>95</v>
       </c>
@@ -1548,7 +1562,7 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="21" t="s">
@@ -1576,7 +1590,7 @@
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="21" t="s">
         <v>68</v>
       </c>
@@ -1595,7 +1609,7 @@
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="21" t="s">
         <v>44</v>
       </c>
@@ -1614,7 +1628,7 @@
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -1626,7 +1640,9 @@
       <c r="D23" s="15">
         <v>3</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="18">
+        <v>3</v>
+      </c>
       <c r="F23" s="21" t="s">
         <v>23</v>
       </c>
@@ -1637,7 +1653,7 @@
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="19"/>
       <c r="C24" s="25"/>
       <c r="D24" s="15"/>
@@ -1653,13 +1669,13 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
+      <c r="A25" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="15" t="s">
         <v>4</v>
       </c>
@@ -1673,11 +1689,11 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="21" t="s">
         <v>11</v>
       </c>
@@ -1689,7 +1705,7 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="41" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="25" t="s">
@@ -1713,7 +1729,7 @@
       <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="25" t="s">
         <v>71</v>
       </c>
@@ -1735,7 +1751,7 @@
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="25" t="s">
         <v>91</v>
       </c>
@@ -1753,7 +1769,7 @@
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="1:10" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="41" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="21" t="s">
@@ -1768,14 +1784,14 @@
       <c r="E30" s="21">
         <v>3</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="1:10" ht="61.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="21" t="s">
         <v>29</v>
       </c>
@@ -1788,14 +1804,14 @@
       <c r="E31" s="21">
         <v>3</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="21" t="s">
         <v>30</v>
       </c>
@@ -1808,24 +1824,24 @@
       <c r="E32" s="21">
         <v>3</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="43" t="s">
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="44" t="s">
+      <c r="G33" s="39" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="15"/>
@@ -1833,61 +1849,61 @@
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="39"/>
       <c r="H34" s="15"/>
       <c r="I34" s="18"/>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
       <c r="H35" s="15"/>
       <c r="I35" s="18"/>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="39"/>
       <c r="H36" s="15"/>
       <c r="I36" s="18"/>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="39"/>
       <c r="H37" s="15"/>
       <c r="I37" s="18"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="A38" s="38"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="39"/>
       <c r="H38" s="15"/>
       <c r="I38" s="18"/>
       <c r="J38" s="7"/>
@@ -1904,7 +1920,7 @@
       </c>
       <c r="E39" s="15">
         <f>SUM(E8:E38)</f>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="3"/>
@@ -1915,6 +1931,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="F30:I32"/>
@@ -1927,14 +1951,6 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
secret done: ruins done; docs partially done. Todo: snowtown, some puzzles, quick end
</commit_message>
<xml_diff>
--- a/doc/大作业自评表.xlsx
+++ b/doc/大作业自评表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\程序设计基础\2024013355_黄添豪\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B63712-CDDC-4D62-9522-5786FADB5E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE15490-814F-40EA-882E-2E29DC1CBDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,6 +840,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -860,21 +875,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1175,17 +1175,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -1205,10 +1205,10 @@
       <c r="A3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="28"/>
       <c r="F3" s="30"/>
       <c r="G3" s="27"/>
@@ -1230,25 +1230,25 @@
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="31" t="s">
         <v>1</v>
       </c>
@@ -1562,7 +1562,7 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="40" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="21" t="s">
@@ -1590,7 +1590,7 @@
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="21" t="s">
         <v>68</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="21" t="s">
         <v>44</v>
       </c>
@@ -1628,7 +1628,7 @@
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="40" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -1653,7 +1653,7 @@
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="19"/>
       <c r="C24" s="25"/>
       <c r="D24" s="15"/>
@@ -1665,17 +1665,19 @@
         <v>98</v>
       </c>
       <c r="H24" s="15"/>
-      <c r="I24" s="18"/>
+      <c r="I24" s="18">
+        <v>5</v>
+      </c>
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="A25" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="15" t="s">
         <v>4</v>
       </c>
@@ -1689,11 +1691,11 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
       <c r="F26" s="21" t="s">
         <v>11</v>
       </c>
@@ -1705,7 +1707,7 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="46" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="25" t="s">
@@ -1717,7 +1719,9 @@
       <c r="D27" s="21">
         <v>4</v>
       </c>
-      <c r="E27" s="25"/>
+      <c r="E27" s="18">
+        <v>4</v>
+      </c>
       <c r="F27" s="21" t="s">
         <v>72</v>
       </c>
@@ -1729,7 +1733,7 @@
       <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="25" t="s">
         <v>71</v>
       </c>
@@ -1739,7 +1743,9 @@
       <c r="D28" s="21">
         <v>4</v>
       </c>
-      <c r="E28" s="25"/>
+      <c r="E28" s="18">
+        <v>4</v>
+      </c>
       <c r="F28" s="18" t="s">
         <v>74</v>
       </c>
@@ -1751,7 +1757,7 @@
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="25" t="s">
         <v>91</v>
       </c>
@@ -1761,7 +1767,9 @@
       <c r="D29" s="21">
         <v>4</v>
       </c>
-      <c r="E29" s="25"/>
+      <c r="E29" s="18">
+        <v>4</v>
+      </c>
       <c r="F29" s="18"/>
       <c r="G29" s="3"/>
       <c r="H29" s="15"/>
@@ -1769,7 +1777,7 @@
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="1:10" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="46" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="21" t="s">
@@ -1784,14 +1792,14 @@
       <c r="E30" s="21">
         <v>3</v>
       </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="1:10" ht="61.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="21" t="s">
         <v>29</v>
       </c>
@@ -1804,14 +1812,14 @@
       <c r="E31" s="21">
         <v>3</v>
       </c>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="21" t="s">
         <v>30</v>
       </c>
@@ -1824,24 +1832,24 @@
       <c r="E32" s="21">
         <v>3</v>
       </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="38" t="s">
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="39" t="s">
+      <c r="G33" s="44" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="15"/>
@@ -1849,61 +1857,61 @@
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="39"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="15"/>
       <c r="I34" s="18"/>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="15"/>
       <c r="I35" s="18"/>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
       <c r="H36" s="15"/>
       <c r="I36" s="18"/>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="39"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="44"/>
       <c r="H37" s="15"/>
       <c r="I37" s="18"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="39"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="44"/>
       <c r="H38" s="15"/>
       <c r="I38" s="18"/>
       <c r="J38" s="7"/>
@@ -1920,7 +1928,7 @@
       </c>
       <c r="E39" s="15">
         <f>SUM(E8:E38)</f>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="3"/>
@@ -1931,14 +1939,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="F30:I32"/>
@@ -1951,6 +1951,14 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>